<commit_message>
feat(benchmarks): Bun on WSL2 but Node.js is very slow
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksOverview.xlsx
+++ b/benchmarks/BenchmarksOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I573017/Documents/Development/Repositories/BunVsNodeJs/benchmarks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C6A3C2-0D4D-1441-A959-E8A57810A4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5D8283-1682-4E2E-92C3-7DB26A0F98B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="-31500" windowWidth="38400" windowHeight="31500" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Setup 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>Test Setup</t>
   </si>
@@ -84,9 +84,6 @@
     <t>System</t>
   </si>
   <si>
-    <t>Win11</t>
-  </si>
-  <si>
     <t>WSL2</t>
   </si>
 </sst>
@@ -94,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,7 +154,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -173,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,28 +466,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E627F5D-FFE4-2643-9D4B-9E18438983C0}">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -498,7 +501,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -506,7 +509,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -526,17 +529,8 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -576,26 +570,8 @@
       <c r="M7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1</v>
       </c>
@@ -617,8 +593,26 @@
       <c r="G8">
         <v>28432</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>113</v>
+      </c>
+      <c r="I8">
+        <v>88376.86</v>
+      </c>
+      <c r="J8">
+        <v>1.41</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>66</v>
+      </c>
+      <c r="M8">
+        <v>80596</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2</v>
       </c>
@@ -640,8 +634,26 @@
       <c r="G9">
         <v>28400</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>111</v>
+      </c>
+      <c r="I9">
+        <v>89640.82</v>
+      </c>
+      <c r="J9">
+        <v>1.39</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>101</v>
+      </c>
+      <c r="M9">
+        <v>70180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3</v>
       </c>
@@ -663,8 +675,26 @@
       <c r="G10">
         <v>28416</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>115</v>
+      </c>
+      <c r="I10">
+        <v>86345.97</v>
+      </c>
+      <c r="J10">
+        <v>1.44</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>105</v>
+      </c>
+      <c r="M10">
+        <v>81500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>4</v>
       </c>
@@ -686,8 +716,26 @@
       <c r="G11">
         <v>28480</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>109</v>
+      </c>
+      <c r="I11">
+        <v>91026.98</v>
+      </c>
+      <c r="J11">
+        <v>1.37</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>104</v>
+      </c>
+      <c r="M11">
+        <v>70028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>5</v>
       </c>
@@ -709,8 +757,26 @@
       <c r="G12">
         <v>28480</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>111</v>
+      </c>
+      <c r="I12">
+        <v>89623.28</v>
+      </c>
+      <c r="J12">
+        <v>1.39</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12">
+        <v>104</v>
+      </c>
+      <c r="M12">
+        <v>72608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>6</v>
       </c>
@@ -732,8 +798,26 @@
       <c r="G13">
         <v>28650</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>103</v>
+      </c>
+      <c r="I13">
+        <v>96231.23</v>
+      </c>
+      <c r="J13">
+        <v>1.3</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13">
+        <v>101</v>
+      </c>
+      <c r="M13">
+        <v>69404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>7</v>
       </c>
@@ -755,8 +839,26 @@
       <c r="G14">
         <v>28304</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>104</v>
+      </c>
+      <c r="I14">
+        <v>95817.84</v>
+      </c>
+      <c r="J14">
+        <v>1.3</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>101</v>
+      </c>
+      <c r="M14">
+        <v>82844</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>8</v>
       </c>
@@ -778,8 +880,26 @@
       <c r="G15">
         <v>28512</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>109</v>
+      </c>
+      <c r="I15">
+        <v>91343.1</v>
+      </c>
+      <c r="J15">
+        <v>1.37</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15">
+        <v>101</v>
+      </c>
+      <c r="M15">
+        <v>69980</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>9</v>
       </c>
@@ -801,8 +921,26 @@
       <c r="G16">
         <v>28560</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>103</v>
+      </c>
+      <c r="I16">
+        <v>96874.27</v>
+      </c>
+      <c r="J16">
+        <v>1.29</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>101</v>
+      </c>
+      <c r="M16">
+        <v>66404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>10</v>
       </c>
@@ -824,8 +962,26 @@
       <c r="G17">
         <v>28480</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>106</v>
+      </c>
+      <c r="I17">
+        <v>93845.51</v>
+      </c>
+      <c r="J17">
+        <v>1.33</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17">
+        <v>101</v>
+      </c>
+      <c r="M17">
+        <v>65872</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -845,17 +1001,8 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
@@ -895,76 +1042,238 @@
       <c r="M20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>193</v>
+      </c>
+      <c r="C21">
+        <v>51715.99</v>
+      </c>
+      <c r="D21">
+        <v>2.42</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>79</v>
+      </c>
+      <c r="G21">
+        <v>84048</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>193</v>
+      </c>
+      <c r="C22">
+        <v>51626.61</v>
+      </c>
+      <c r="D22">
+        <v>2.42</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>78</v>
+      </c>
+      <c r="G22">
+        <v>83104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>194</v>
+      </c>
+      <c r="C23">
+        <v>51499.01</v>
+      </c>
+      <c r="D23">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>81</v>
+      </c>
+      <c r="G23">
+        <v>84496</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>193</v>
+      </c>
+      <c r="C24">
+        <v>51575.94</v>
+      </c>
+      <c r="D24">
+        <v>2.42</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>79</v>
+      </c>
+      <c r="G24">
+        <v>84928</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>193</v>
+      </c>
+      <c r="C25">
+        <v>51715.89</v>
+      </c>
+      <c r="D25">
+        <v>2.42</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>82</v>
+      </c>
+      <c r="G25">
+        <v>83584</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>193</v>
+      </c>
+      <c r="C26">
+        <v>51751.95</v>
+      </c>
+      <c r="D26">
+        <v>2.41</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>82</v>
+      </c>
+      <c r="G26">
+        <v>84336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>193</v>
+      </c>
+      <c r="C27">
+        <v>51739.01</v>
+      </c>
+      <c r="D27">
+        <v>2.31</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>81</v>
+      </c>
+      <c r="G27">
+        <v>84624</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>193</v>
+      </c>
+      <c r="C28">
+        <v>51832.58</v>
+      </c>
+      <c r="D28">
+        <v>2.41</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>82</v>
+      </c>
+      <c r="G28">
+        <v>84096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>193</v>
+      </c>
+      <c r="C29">
+        <v>51581.57</v>
+      </c>
+      <c r="D29">
+        <v>2.42</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29">
+        <v>80</v>
+      </c>
+      <c r="G29">
+        <v>83648</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>197</v>
+      </c>
+      <c r="C30">
+        <v>50706.23</v>
+      </c>
+      <c r="D30">
+        <v>2.46</v>
+      </c>
+      <c r="E30">
+        <v>100</v>
+      </c>
+      <c r="F30">
+        <v>85</v>
+      </c>
+      <c r="G30">
+        <v>83246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -984,17 +1293,8 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -1034,86 +1334,245 @@
       <c r="M33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S33" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>187</v>
+      </c>
+      <c r="C34">
+        <v>53397.98</v>
+      </c>
+      <c r="D34">
+        <v>2.34</v>
+      </c>
+      <c r="E34">
+        <v>100</v>
+      </c>
+      <c r="F34">
+        <v>82</v>
+      </c>
+      <c r="G34">
+        <v>79088</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>189</v>
+      </c>
+      <c r="C35">
+        <v>52817.16</v>
+      </c>
+      <c r="D35">
+        <v>2.37</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35">
+        <v>82</v>
+      </c>
+      <c r="G35">
+        <v>79520</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>191</v>
+      </c>
+      <c r="C36">
+        <v>52188.49</v>
+      </c>
+      <c r="D36">
+        <v>2.39</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36">
+        <v>85</v>
+      </c>
+      <c r="G36">
+        <v>79840</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>188</v>
+      </c>
+      <c r="C37">
+        <v>53005.33</v>
+      </c>
+      <c r="D37">
+        <v>2.36</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37">
+        <v>76</v>
+      </c>
+      <c r="G37">
+        <v>79136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>187</v>
+      </c>
+      <c r="C38">
+        <v>53467.01</v>
+      </c>
+      <c r="D38">
+        <v>2.34</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38">
+        <v>83</v>
+      </c>
+      <c r="G38">
+        <v>78544</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>188</v>
+      </c>
+      <c r="C39">
+        <v>52967.96</v>
+      </c>
+      <c r="D39">
+        <v>2.36</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39">
+        <v>83</v>
+      </c>
+      <c r="G39">
+        <v>78736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>189</v>
+      </c>
+      <c r="C40">
+        <v>52839.1</v>
+      </c>
+      <c r="D40">
+        <v>2.37</v>
+      </c>
+      <c r="E40">
+        <v>100</v>
+      </c>
+      <c r="F40">
+        <v>84</v>
+      </c>
+      <c r="G40">
+        <v>79296</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>189</v>
+      </c>
+      <c r="C41">
+        <v>52799.25</v>
+      </c>
+      <c r="D41">
+        <v>2.37</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41">
+        <v>84</v>
+      </c>
+      <c r="G41">
+        <v>78384</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>190</v>
+      </c>
+      <c r="C42">
+        <v>52589.67</v>
+      </c>
+      <c r="D42">
+        <v>2.38</v>
+      </c>
+      <c r="E42">
+        <v>100</v>
+      </c>
+      <c r="F42">
+        <v>81</v>
+      </c>
+      <c r="G42">
+        <v>78960</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43">
         <v>10</v>
       </c>
+      <c r="B43">
+        <v>189</v>
+      </c>
+      <c r="C43">
+        <v>52739.19</v>
+      </c>
+      <c r="D43">
+        <v>2.37</v>
+      </c>
+      <c r="E43">
+        <v>100</v>
+      </c>
+      <c r="F43">
+        <v>83</v>
+      </c>
+      <c r="G43">
+        <v>78960</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="6">
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B32:G32"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="H19:N19"/>
-    <mergeCell ref="O19:T19"/>
-    <mergeCell ref="H32:N32"/>
-    <mergeCell ref="O32:T32"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="H32:M32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1126,9 +1585,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
feat(benchmarks): lastvergleich file server finished
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksOverview.xlsx
+++ b/benchmarks/BenchmarksOverview.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I573017/Documents/Development/Repositories/BunVsNodeJs/benchmarks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A726241-FFF1-D041-BEC1-16A529F6AD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF6B1F4-20D1-40B4-A48B-99C2148CCD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic HTTP Server" sheetId="1" r:id="rId1"/>
-    <sheet name="File Server" sheetId="2" r:id="rId2"/>
-    <sheet name="File Server Lastvergleich" sheetId="4" r:id="rId3"/>
-    <sheet name="Fibonacci" sheetId="3" r:id="rId4"/>
+    <sheet name="File Server Lastvergleich" sheetId="4" r:id="rId2"/>
+    <sheet name="Fibonacci" sheetId="3" r:id="rId3"/>
+    <sheet name="File Server" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,7 +176,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -494,39 +494,39 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -543,7 +543,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -584,7 +584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1</v>
       </c>
@@ -625,7 +625,7 @@
         <v>47188</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2</v>
       </c>
@@ -666,7 +666,7 @@
         <v>47608</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3</v>
       </c>
@@ -707,7 +707,7 @@
         <v>49392</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>4</v>
       </c>
@@ -748,7 +748,7 @@
         <v>47260</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>5</v>
       </c>
@@ -789,7 +789,7 @@
         <v>48484</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -847,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>1</v>
       </c>
@@ -888,7 +888,7 @@
         <v>93856</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>2</v>
       </c>
@@ -929,7 +929,7 @@
         <v>93212</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>3</v>
       </c>
@@ -970,7 +970,7 @@
         <v>93144</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>92928</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>93116</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>86652</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>86396</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>86280</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>86284</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>5</v>
       </c>
@@ -1330,991 +1330,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506776CC-B6C8-BB4A-88D0-81938826640D}">
-  <dimension ref="A1:M28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>500</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5">
-        <v>30</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>23707.59</v>
-      </c>
-      <c r="C8">
-        <v>21.08</v>
-      </c>
-      <c r="D8">
-        <v>195.63</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>90</v>
-      </c>
-      <c r="G8">
-        <v>64264</v>
-      </c>
-      <c r="H8" s="2">
-        <v>23899.18</v>
-      </c>
-      <c r="I8" s="6">
-        <v>20.91</v>
-      </c>
-      <c r="J8" s="6">
-        <v>116.19</v>
-      </c>
-      <c r="K8" s="5">
-        <v>100</v>
-      </c>
-      <c r="L8" s="5">
-        <v>96</v>
-      </c>
-      <c r="M8" s="5">
-        <v>82128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5">
-        <v>23920.81</v>
-      </c>
-      <c r="C9" s="5">
-        <v>20.9</v>
-      </c>
-      <c r="D9" s="5">
-        <v>239.5</v>
-      </c>
-      <c r="E9" s="5">
-        <v>100</v>
-      </c>
-      <c r="F9" s="5">
-        <v>86</v>
-      </c>
-      <c r="G9" s="5">
-        <v>65040</v>
-      </c>
-      <c r="H9" s="5">
-        <v>24201.74</v>
-      </c>
-      <c r="I9" s="5">
-        <v>20.65</v>
-      </c>
-      <c r="J9" s="5">
-        <v>108.4</v>
-      </c>
-      <c r="K9" s="5">
-        <v>100</v>
-      </c>
-      <c r="L9" s="5">
-        <v>96</v>
-      </c>
-      <c r="M9" s="5">
-        <v>83196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5">
-        <v>23909.89</v>
-      </c>
-      <c r="C10" s="5">
-        <v>20.9</v>
-      </c>
-      <c r="D10" s="5">
-        <v>204.46</v>
-      </c>
-      <c r="E10" s="5">
-        <v>100</v>
-      </c>
-      <c r="F10" s="5">
-        <v>90</v>
-      </c>
-      <c r="G10" s="5">
-        <v>65024</v>
-      </c>
-      <c r="H10" s="5">
-        <v>24153.93</v>
-      </c>
-      <c r="I10" s="5">
-        <v>20.69</v>
-      </c>
-      <c r="J10" s="5">
-        <v>115.38</v>
-      </c>
-      <c r="K10" s="5">
-        <v>100</v>
-      </c>
-      <c r="L10" s="5">
-        <v>100</v>
-      </c>
-      <c r="M10" s="5">
-        <v>82692</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5">
-        <v>23825.78</v>
-      </c>
-      <c r="C11" s="5">
-        <v>20.98</v>
-      </c>
-      <c r="D11" s="5">
-        <v>206.59</v>
-      </c>
-      <c r="E11" s="5">
-        <v>100</v>
-      </c>
-      <c r="F11" s="5">
-        <v>89</v>
-      </c>
-      <c r="G11" s="5">
-        <v>64880</v>
-      </c>
-      <c r="H11" s="5">
-        <v>23658.7</v>
-      </c>
-      <c r="I11" s="5">
-        <v>21.12</v>
-      </c>
-      <c r="J11" s="5">
-        <v>119.64</v>
-      </c>
-      <c r="K11" s="5">
-        <v>100</v>
-      </c>
-      <c r="L11" s="5">
-        <v>98</v>
-      </c>
-      <c r="M11" s="5">
-        <v>82672</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>5</v>
-      </c>
-      <c r="B12" s="5">
-        <v>23879.56</v>
-      </c>
-      <c r="C12" s="5">
-        <v>20.93</v>
-      </c>
-      <c r="D12" s="5">
-        <v>220.08</v>
-      </c>
-      <c r="E12" s="5">
-        <v>100</v>
-      </c>
-      <c r="F12" s="5">
-        <v>90</v>
-      </c>
-      <c r="G12" s="5">
-        <v>64880</v>
-      </c>
-      <c r="H12" s="5">
-        <v>24399.08</v>
-      </c>
-      <c r="I12" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="J12" s="5">
-        <v>117.62</v>
-      </c>
-      <c r="K12" s="5">
-        <v>100</v>
-      </c>
-      <c r="L12" s="5">
-        <v>99</v>
-      </c>
-      <c r="M12" s="5">
-        <v>82948</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5">
-        <v>24363.11</v>
-      </c>
-      <c r="I13" s="5">
-        <v>20.51</v>
-      </c>
-      <c r="J13" s="5">
-        <v>120.77</v>
-      </c>
-      <c r="K13" s="5">
-        <v>100</v>
-      </c>
-      <c r="L13" s="5">
-        <v>99</v>
-      </c>
-      <c r="M13" s="5">
-        <v>84116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5">
-        <v>14317.65</v>
-      </c>
-      <c r="C16" s="5">
-        <v>34.93</v>
-      </c>
-      <c r="D16" s="5">
-        <v>248.08</v>
-      </c>
-      <c r="E16" s="5">
-        <v>100</v>
-      </c>
-      <c r="F16" s="5">
-        <v>189</v>
-      </c>
-      <c r="G16" s="5">
-        <v>229776</v>
-      </c>
-      <c r="H16" s="5">
-        <v>7650.31</v>
-      </c>
-      <c r="I16" s="5">
-        <v>64.53</v>
-      </c>
-      <c r="J16" s="5">
-        <v>287.7</v>
-      </c>
-      <c r="K16" s="5">
-        <v>100</v>
-      </c>
-      <c r="L16" s="5">
-        <v>166</v>
-      </c>
-      <c r="M16" s="5">
-        <v>105356</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-      <c r="B17" s="5">
-        <v>14508.2</v>
-      </c>
-      <c r="C17" s="5">
-        <v>34.46</v>
-      </c>
-      <c r="D17" s="5">
-        <v>231.62</v>
-      </c>
-      <c r="E17" s="5">
-        <v>100</v>
-      </c>
-      <c r="F17" s="5">
-        <v>197</v>
-      </c>
-      <c r="G17" s="5">
-        <v>198496</v>
-      </c>
-      <c r="H17" s="5">
-        <v>8460.4599999999991</v>
-      </c>
-      <c r="I17" s="5">
-        <v>58.41</v>
-      </c>
-      <c r="J17" s="5">
-        <v>305.45999999999998</v>
-      </c>
-      <c r="K17" s="5">
-        <v>100</v>
-      </c>
-      <c r="L17" s="5">
-        <v>176</v>
-      </c>
-      <c r="M17" s="5">
-        <v>106928</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>3</v>
-      </c>
-      <c r="B18" s="5">
-        <v>14466.72</v>
-      </c>
-      <c r="C18" s="5">
-        <v>34.56</v>
-      </c>
-      <c r="D18" s="5">
-        <v>214.82</v>
-      </c>
-      <c r="E18" s="5">
-        <v>100</v>
-      </c>
-      <c r="F18" s="5">
-        <v>185</v>
-      </c>
-      <c r="G18" s="5">
-        <v>208496</v>
-      </c>
-      <c r="H18" s="5">
-        <v>8428.35</v>
-      </c>
-      <c r="I18" s="5">
-        <v>58.51</v>
-      </c>
-      <c r="J18" s="5">
-        <v>285.69</v>
-      </c>
-      <c r="K18" s="5">
-        <v>100</v>
-      </c>
-      <c r="L18" s="5">
-        <v>166</v>
-      </c>
-      <c r="M18" s="5">
-        <v>103704</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>4</v>
-      </c>
-      <c r="B19" s="5">
-        <v>14610.55</v>
-      </c>
-      <c r="C19" s="5">
-        <v>34.21</v>
-      </c>
-      <c r="D19" s="5">
-        <v>198.59</v>
-      </c>
-      <c r="E19" s="5">
-        <v>100</v>
-      </c>
-      <c r="F19" s="5">
-        <v>176</v>
-      </c>
-      <c r="G19" s="5">
-        <v>212880</v>
-      </c>
-      <c r="H19" s="5">
-        <v>8292.3700000000008</v>
-      </c>
-      <c r="I19" s="5">
-        <v>59.61</v>
-      </c>
-      <c r="J19" s="5">
-        <v>313.20999999999998</v>
-      </c>
-      <c r="K19" s="5">
-        <v>100</v>
-      </c>
-      <c r="L19" s="5">
-        <v>171</v>
-      </c>
-      <c r="M19" s="5">
-        <v>106108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>5</v>
-      </c>
-      <c r="B20" s="5">
-        <v>14647.9</v>
-      </c>
-      <c r="C20" s="5">
-        <v>34.119999999999997</v>
-      </c>
-      <c r="D20" s="5">
-        <v>238.61</v>
-      </c>
-      <c r="E20" s="5">
-        <v>100</v>
-      </c>
-      <c r="F20" s="5">
-        <v>190</v>
-      </c>
-      <c r="G20" s="5">
-        <v>209896</v>
-      </c>
-      <c r="H20" s="5">
-        <v>8410.83</v>
-      </c>
-      <c r="I20" s="5">
-        <v>58.73</v>
-      </c>
-      <c r="J20" s="5">
-        <v>292.88</v>
-      </c>
-      <c r="K20" s="5">
-        <v>100</v>
-      </c>
-      <c r="L20" s="5">
-        <v>165</v>
-      </c>
-      <c r="M20" s="5">
-        <v>104264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>1</v>
-      </c>
-      <c r="B24" s="5">
-        <v>14790.27</v>
-      </c>
-      <c r="C24" s="5">
-        <v>33.81</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1720</v>
-      </c>
-      <c r="E24" s="5">
-        <v>99.5</v>
-      </c>
-      <c r="F24" s="5">
-        <v>195</v>
-      </c>
-      <c r="G24" s="5">
-        <v>221728</v>
-      </c>
-      <c r="H24" s="5">
-        <v>10322.75</v>
-      </c>
-      <c r="I24" s="5">
-        <v>47.96</v>
-      </c>
-      <c r="J24" s="5">
-        <v>1710</v>
-      </c>
-      <c r="K24" s="5">
-        <v>100</v>
-      </c>
-      <c r="L24" s="5">
-        <v>268</v>
-      </c>
-      <c r="M24" s="5">
-        <v>172996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
-        <v>2</v>
-      </c>
-      <c r="B25" s="5">
-        <v>14729.2</v>
-      </c>
-      <c r="C25" s="5">
-        <v>33.93</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1790</v>
-      </c>
-      <c r="E25" s="5">
-        <v>99.4</v>
-      </c>
-      <c r="F25" s="5">
-        <v>194</v>
-      </c>
-      <c r="G25" s="5">
-        <v>219552</v>
-      </c>
-      <c r="H25" s="5">
-        <v>10462.030000000001</v>
-      </c>
-      <c r="I25" s="5">
-        <v>47.33</v>
-      </c>
-      <c r="J25" s="5">
-        <v>1740</v>
-      </c>
-      <c r="K25" s="5">
-        <v>100</v>
-      </c>
-      <c r="L25" s="5">
-        <v>265</v>
-      </c>
-      <c r="M25" s="5">
-        <v>118604</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
-        <v>3</v>
-      </c>
-      <c r="B26" s="5">
-        <v>14749.95</v>
-      </c>
-      <c r="C26" s="5">
-        <v>33.909999999999997</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1649</v>
-      </c>
-      <c r="E26" s="5">
-        <v>99.7</v>
-      </c>
-      <c r="F26" s="5">
-        <v>198</v>
-      </c>
-      <c r="G26" s="5">
-        <v>234800</v>
-      </c>
-      <c r="H26" s="5">
-        <v>10337.76</v>
-      </c>
-      <c r="I26" s="5">
-        <v>47.97</v>
-      </c>
-      <c r="J26" s="5">
-        <v>1770</v>
-      </c>
-      <c r="K26" s="5">
-        <v>100</v>
-      </c>
-      <c r="L26" s="5">
-        <v>250</v>
-      </c>
-      <c r="M26" s="5">
-        <v>174576</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
-        <v>4</v>
-      </c>
-      <c r="B27" s="5">
-        <v>14722.22</v>
-      </c>
-      <c r="C27" s="5">
-        <v>33.979999999999997</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1920</v>
-      </c>
-      <c r="E27" s="5">
-        <v>99.4</v>
-      </c>
-      <c r="F27" s="5">
-        <v>193</v>
-      </c>
-      <c r="G27" s="5">
-        <v>243920</v>
-      </c>
-      <c r="H27" s="5">
-        <v>10478.85</v>
-      </c>
-      <c r="I27" s="5">
-        <v>47.32</v>
-      </c>
-      <c r="J27" s="5">
-        <v>1740</v>
-      </c>
-      <c r="K27" s="5">
-        <v>100</v>
-      </c>
-      <c r="L27" s="5">
-        <v>264</v>
-      </c>
-      <c r="M27" s="5">
-        <v>175628</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="5">
-        <v>5</v>
-      </c>
-      <c r="B28" s="5">
-        <v>14628.28</v>
-      </c>
-      <c r="C28" s="5">
-        <v>34.14</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1820</v>
-      </c>
-      <c r="E28" s="5">
-        <v>99.7</v>
-      </c>
-      <c r="F28" s="5">
-        <v>194</v>
-      </c>
-      <c r="G28" s="5">
-        <v>257200</v>
-      </c>
-      <c r="H28" s="5">
-        <v>10254</v>
-      </c>
-      <c r="I28" s="5">
-        <v>48.39</v>
-      </c>
-      <c r="J28" s="5">
-        <v>1740</v>
-      </c>
-      <c r="K28" s="5">
-        <v>100</v>
-      </c>
-      <c r="L28" s="5">
-        <v>262</v>
-      </c>
-      <c r="M28" s="5">
-        <v>175036</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="H22:M22"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB541521-64F8-DE46-A0B5-E150B1049D8B}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="87" workbookViewId="0">
-      <selection activeCell="O64" sqref="O64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -2322,7 +1356,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23">
       <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
@@ -2352,7 +1386,7 @@
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2387,7 +1421,7 @@
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7" s="4">
         <v>50</v>
       </c>
@@ -2452,7 +1486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -2517,7 +1551,7 @@
         <v>88056</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -2582,7 +1616,7 @@
         <v>84784</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -2647,7 +1681,7 @@
         <v>82028</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -2712,7 +1746,7 @@
         <v>85144</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -2777,7 +1811,7 @@
         <v>86808</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2800,7 +1834,7 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2835,7 +1869,7 @@
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23">
       <c r="A15" s="4">
         <v>250</v>
       </c>
@@ -2900,7 +1934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23">
       <c r="A16" s="5">
         <v>1</v>
       </c>
@@ -2965,7 +1999,7 @@
         <v>128460</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="A17" s="5">
         <v>2</v>
       </c>
@@ -3030,7 +2064,7 @@
         <v>124552</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="A18" s="5">
         <v>3</v>
       </c>
@@ -3095,7 +2129,7 @@
         <v>121192</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="A19" s="5">
         <v>4</v>
       </c>
@@ -3160,7 +2194,7 @@
         <v>121700</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23">
       <c r="A20" s="5">
         <v>5</v>
       </c>
@@ -3225,7 +2259,7 @@
         <v>121488</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3248,7 +2282,7 @@
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
@@ -3283,7 +2317,7 @@
       <c r="V22" s="8"/>
       <c r="W22" s="8"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23">
       <c r="A23" s="4">
         <v>500</v>
       </c>
@@ -3348,7 +2382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23">
       <c r="A24" s="5">
         <v>1</v>
       </c>
@@ -3413,7 +2447,7 @@
         <v>172996</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23">
       <c r="A25" s="5">
         <v>2</v>
       </c>
@@ -3478,7 +2512,7 @@
         <v>118604</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23">
       <c r="A26" s="5">
         <v>3</v>
       </c>
@@ -3543,7 +2577,7 @@
         <v>174576</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23">
       <c r="A27" s="5">
         <v>4</v>
       </c>
@@ -3608,7 +2642,7 @@
         <v>175628</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23">
       <c r="A28" s="5">
         <v>5</v>
       </c>
@@ -3673,7 +2707,7 @@
         <v>175036</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23">
       <c r="B29" s="5">
         <v>24363.11</v>
       </c>
@@ -3693,7 +2727,7 @@
         <v>84116</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23">
       <c r="A30" s="4" t="s">
         <v>9</v>
       </c>
@@ -3728,7 +2762,7 @@
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23">
       <c r="A31" s="4">
         <v>1000</v>
       </c>
@@ -3793,7 +2827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23">
       <c r="A32" s="5">
         <v>1</v>
       </c>
@@ -3858,7 +2892,7 @@
         <v>213864</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23">
       <c r="A33" s="5">
         <v>2</v>
       </c>
@@ -3923,7 +2957,7 @@
         <v>209776</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23">
       <c r="A34" s="5">
         <v>3</v>
       </c>
@@ -3988,7 +3022,7 @@
         <v>209276</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23">
       <c r="A35" s="5">
         <v>4</v>
       </c>
@@ -4053,7 +3087,7 @@
         <v>211692</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23">
       <c r="A36" s="5">
         <v>5</v>
       </c>
@@ -4118,7 +3152,7 @@
         <v>213220</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23">
       <c r="A40" s="9" t="s">
         <v>2</v>
       </c>
@@ -4148,12 +3182,12 @@
       <c r="V40" s="9"/>
       <c r="W40" s="9"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23">
       <c r="A41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -4164,7 +3198,7 @@
         <v>9</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -4175,7 +3209,7 @@
         <v>9</v>
       </c>
       <c r="R41" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
@@ -4183,7 +3217,7 @@
       <c r="V41" s="8"/>
       <c r="W41" s="8"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23">
       <c r="A42" s="4">
         <v>50</v>
       </c>
@@ -4248,134 +3282,332 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23">
       <c r="A43" s="5">
         <v>1</v>
       </c>
+      <c r="B43">
+        <v>25276.77</v>
+      </c>
+      <c r="C43">
+        <v>1.98</v>
+      </c>
+      <c r="D43">
+        <v>18.82</v>
+      </c>
+      <c r="E43">
+        <v>100</v>
+      </c>
+      <c r="F43">
+        <v>92</v>
+      </c>
+      <c r="G43">
+        <v>67328</v>
+      </c>
       <c r="I43" s="5">
         <v>1</v>
       </c>
+      <c r="J43">
+        <v>21515</v>
+      </c>
+      <c r="K43">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="L43">
+        <v>33.96</v>
+      </c>
+      <c r="M43">
+        <v>100</v>
+      </c>
+      <c r="N43">
+        <v>146</v>
+      </c>
+      <c r="O43">
+        <v>120544</v>
+      </c>
       <c r="Q43" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R43">
+        <v>21553.66</v>
+      </c>
+      <c r="S43">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="T43">
+        <v>81.25</v>
+      </c>
+      <c r="U43">
+        <v>100</v>
+      </c>
+      <c r="V43">
+        <v>146</v>
+      </c>
+      <c r="W43">
+        <v>117296</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
       <c r="A44" s="5">
         <v>2</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="B44" s="5">
+        <v>25302.77</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1.97</v>
+      </c>
+      <c r="D44" s="5">
+        <v>14.4</v>
+      </c>
+      <c r="E44" s="5">
+        <v>100</v>
+      </c>
+      <c r="F44" s="5">
+        <v>94</v>
+      </c>
+      <c r="G44" s="5">
+        <v>65744</v>
+      </c>
       <c r="I44" s="5">
         <v>2</v>
       </c>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
+      <c r="J44" s="5">
+        <v>19785.3</v>
+      </c>
+      <c r="K44" s="5">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="L44" s="5">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="M44" s="5">
+        <v>100</v>
+      </c>
+      <c r="N44" s="5">
+        <v>142</v>
+      </c>
+      <c r="O44" s="5">
+        <v>125616</v>
+      </c>
       <c r="Q44" s="5">
         <v>2</v>
       </c>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="5"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R44" s="5">
+        <v>21499.51</v>
+      </c>
+      <c r="S44" s="5">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="T44" s="5">
+        <v>61.8</v>
+      </c>
+      <c r="U44" s="5">
+        <v>100</v>
+      </c>
+      <c r="V44" s="5">
+        <v>148</v>
+      </c>
+      <c r="W44" s="5">
+        <v>109888</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
       <c r="A45" s="5">
         <v>3</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="B45" s="5">
+        <v>25293.360000000001</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1.98</v>
+      </c>
+      <c r="D45" s="5">
+        <v>14.06</v>
+      </c>
+      <c r="E45" s="5">
+        <v>100</v>
+      </c>
+      <c r="F45" s="5">
+        <v>95</v>
+      </c>
+      <c r="G45" s="5">
+        <v>65840</v>
+      </c>
       <c r="I45" s="5">
         <v>3</v>
       </c>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
+      <c r="J45" s="5">
+        <v>19363.939999999999</v>
+      </c>
+      <c r="K45" s="5">
+        <v>2.58</v>
+      </c>
+      <c r="L45" s="5">
+        <v>33.9</v>
+      </c>
+      <c r="M45" s="5">
+        <v>100</v>
+      </c>
+      <c r="N45" s="5">
+        <v>143</v>
+      </c>
+      <c r="O45" s="5">
+        <v>124096</v>
+      </c>
       <c r="Q45" s="5">
         <v>3</v>
       </c>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
-      <c r="W45" s="5"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R45" s="5">
+        <v>21808.63</v>
+      </c>
+      <c r="S45" s="5">
+        <v>2.29</v>
+      </c>
+      <c r="T45" s="5">
+        <v>61.93</v>
+      </c>
+      <c r="U45" s="5">
+        <v>100</v>
+      </c>
+      <c r="V45" s="5">
+        <v>146</v>
+      </c>
+      <c r="W45" s="5">
+        <v>112464</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
       <c r="A46" s="5">
         <v>4</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="B46" s="5">
+        <v>25292.46</v>
+      </c>
+      <c r="C46" s="5">
+        <v>1.98</v>
+      </c>
+      <c r="D46" s="5">
+        <v>13.51</v>
+      </c>
+      <c r="E46" s="5">
+        <v>100</v>
+      </c>
+      <c r="F46" s="5">
+        <v>93</v>
+      </c>
+      <c r="G46" s="5">
+        <v>65956</v>
+      </c>
       <c r="I46" s="5">
         <v>4</v>
       </c>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
+      <c r="J46" s="5">
+        <v>21722.080000000002</v>
+      </c>
+      <c r="K46" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L46" s="5">
+        <v>29.84</v>
+      </c>
+      <c r="M46" s="5">
+        <v>100</v>
+      </c>
+      <c r="N46" s="5">
+        <v>143</v>
+      </c>
+      <c r="O46" s="5">
+        <v>109568</v>
+      </c>
       <c r="Q46" s="5">
         <v>4</v>
       </c>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5"/>
-      <c r="W46" s="5"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R46" s="5">
+        <v>21799.37</v>
+      </c>
+      <c r="S46" s="5">
+        <v>2.29</v>
+      </c>
+      <c r="T46" s="5">
+        <v>63.66</v>
+      </c>
+      <c r="U46" s="5">
+        <v>100</v>
+      </c>
+      <c r="V46" s="5">
+        <v>144</v>
+      </c>
+      <c r="W46" s="5">
+        <v>119520</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23">
       <c r="A47" s="5">
         <v>5</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="B47" s="5">
+        <v>25330.78</v>
+      </c>
+      <c r="C47" s="5">
+        <v>1.97</v>
+      </c>
+      <c r="D47" s="5">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E47" s="5">
+        <v>100</v>
+      </c>
+      <c r="F47" s="5">
+        <v>94</v>
+      </c>
+      <c r="G47" s="5">
+        <v>654230</v>
+      </c>
       <c r="I47" s="5">
         <v>5</v>
       </c>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
+      <c r="J47" s="5">
+        <v>21449.79</v>
+      </c>
+      <c r="K47" s="5">
+        <v>2.33</v>
+      </c>
+      <c r="L47" s="5">
+        <v>33.51</v>
+      </c>
+      <c r="M47" s="5">
+        <v>100</v>
+      </c>
+      <c r="N47" s="5">
+        <v>145</v>
+      </c>
+      <c r="O47" s="5">
+        <v>119792</v>
+      </c>
       <c r="Q47" s="5">
         <v>5</v>
       </c>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R47" s="5">
+        <v>21519.05</v>
+      </c>
+      <c r="S47" s="5">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="T47" s="5">
+        <v>60.17</v>
+      </c>
+      <c r="U47" s="5">
+        <v>100</v>
+      </c>
+      <c r="V47" s="5">
+        <v>148</v>
+      </c>
+      <c r="W47" s="5">
+        <v>115120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -4398,12 +3630,12 @@
       <c r="V48" s="5"/>
       <c r="W48" s="5"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23">
       <c r="A49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4414,7 +3646,7 @@
         <v>9</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
@@ -4425,7 +3657,7 @@
         <v>9</v>
       </c>
       <c r="R49" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="S49" s="8"/>
       <c r="T49" s="8"/>
@@ -4433,7 +3665,7 @@
       <c r="V49" s="8"/>
       <c r="W49" s="8"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23">
       <c r="A50" s="4">
         <v>250</v>
       </c>
@@ -4498,152 +3730,337 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23">
       <c r="A51" s="5">
         <v>1</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="B51" s="5">
+        <v>25464.61</v>
+      </c>
+      <c r="C51" s="5">
+        <v>9.82</v>
+      </c>
+      <c r="D51" s="5">
+        <v>55.58</v>
+      </c>
+      <c r="E51" s="5">
+        <v>100</v>
+      </c>
+      <c r="F51" s="5">
+        <v>89</v>
+      </c>
+      <c r="G51" s="5">
+        <v>66698</v>
+      </c>
       <c r="I51" s="5">
         <v>1</v>
       </c>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
+      <c r="J51" s="5">
+        <v>15917.54</v>
+      </c>
+      <c r="K51" s="5">
+        <v>15.55</v>
+      </c>
+      <c r="L51" s="5">
+        <v>70.349999999999994</v>
+      </c>
+      <c r="M51" s="5">
+        <v>100</v>
+      </c>
+      <c r="N51" s="5">
+        <v>193</v>
+      </c>
+      <c r="O51" s="5">
+        <v>195552</v>
+      </c>
       <c r="Q51" s="5">
         <v>1</v>
       </c>
-      <c r="R51" s="5"/>
-      <c r="S51" s="5"/>
-      <c r="T51" s="5"/>
-      <c r="U51" s="5"/>
-      <c r="V51" s="5"/>
-      <c r="W51" s="5"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R51" s="5">
+        <v>17388.28</v>
+      </c>
+      <c r="S51" s="5">
+        <v>14.38</v>
+      </c>
+      <c r="T51" s="5">
+        <v>469.75</v>
+      </c>
+      <c r="U51" s="6">
+        <f>100-48/(48+521755)*100</f>
+        <v>99.990801126095477</v>
+      </c>
+      <c r="V51" s="5">
+        <v>190</v>
+      </c>
+      <c r="W51" s="5">
+        <v>203264</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
       <c r="A52" s="5">
         <v>2</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="B52" s="5">
+        <v>25435.68</v>
+      </c>
+      <c r="C52" s="5">
+        <v>9.83</v>
+      </c>
+      <c r="D52" s="5">
+        <v>52.12</v>
+      </c>
+      <c r="E52" s="5">
+        <v>100</v>
+      </c>
+      <c r="F52" s="5">
+        <v>92</v>
+      </c>
+      <c r="G52" s="5">
+        <v>66384</v>
+      </c>
       <c r="I52" s="5">
         <v>2</v>
       </c>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
+      <c r="J52" s="5">
+        <v>16075.37</v>
+      </c>
+      <c r="K52" s="5">
+        <v>15.51</v>
+      </c>
+      <c r="L52" s="5">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="M52" s="5">
+        <v>100</v>
+      </c>
+      <c r="N52" s="5">
+        <v>186</v>
+      </c>
+      <c r="O52" s="5">
+        <v>168992</v>
+      </c>
       <c r="Q52" s="5">
         <v>2</v>
       </c>
-      <c r="R52" s="5"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
-      <c r="V52" s="5"/>
-      <c r="W52" s="5"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R52" s="5">
+        <v>17301.54</v>
+      </c>
+      <c r="S52" s="5">
+        <v>14.45</v>
+      </c>
+      <c r="T52" s="5">
+        <v>484.46</v>
+      </c>
+      <c r="U52" s="6">
+        <f>100-42/(42+519209)*100</f>
+        <v>99.991911426265915</v>
+      </c>
+      <c r="V52" s="5">
+        <v>191</v>
+      </c>
+      <c r="W52" s="5">
+        <v>202544</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23">
       <c r="A53" s="5">
         <v>3</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="B53" s="5">
+        <v>25476.74</v>
+      </c>
+      <c r="C53" s="5">
+        <v>9.81</v>
+      </c>
+      <c r="D53" s="5">
+        <v>50.91</v>
+      </c>
+      <c r="E53" s="5">
+        <v>100</v>
+      </c>
+      <c r="F53" s="5">
+        <v>93</v>
+      </c>
+      <c r="G53" s="5">
+        <v>66464</v>
+      </c>
       <c r="I53" s="5">
         <v>3</v>
       </c>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
+      <c r="J53" s="5">
+        <v>16074.26</v>
+      </c>
+      <c r="K53" s="5">
+        <v>15.55</v>
+      </c>
+      <c r="L53" s="5">
+        <v>65.209999999999994</v>
+      </c>
+      <c r="M53" s="5">
+        <v>100</v>
+      </c>
+      <c r="N53" s="5">
+        <v>189</v>
+      </c>
+      <c r="O53" s="5">
+        <v>191920</v>
+      </c>
       <c r="Q53" s="5">
         <v>3</v>
       </c>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="5"/>
-      <c r="U53" s="5"/>
-      <c r="V53" s="5"/>
-      <c r="W53" s="5"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R53" s="5">
+        <v>17374.5</v>
+      </c>
+      <c r="S53" s="5">
+        <v>14.39</v>
+      </c>
+      <c r="T53" s="5">
+        <v>455.17</v>
+      </c>
+      <c r="U53" s="6">
+        <f>100-26/(26+521380)*100</f>
+        <v>99.99501348277542</v>
+      </c>
+      <c r="V53" s="5">
+        <v>186</v>
+      </c>
+      <c r="W53" s="5">
+        <v>184224</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23">
       <c r="A54" s="5">
         <v>4</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="B54" s="5">
+        <v>25372.19</v>
+      </c>
+      <c r="C54" s="5">
+        <v>9.85</v>
+      </c>
+      <c r="D54" s="5">
+        <v>49.03</v>
+      </c>
+      <c r="E54" s="5">
+        <v>100</v>
+      </c>
+      <c r="F54" s="5">
+        <v>92</v>
+      </c>
+      <c r="G54" s="5">
+        <v>66640</v>
+      </c>
       <c r="I54" s="5">
         <v>4</v>
       </c>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
+      <c r="J54" s="5">
+        <v>16111.43</v>
+      </c>
+      <c r="K54" s="5">
+        <v>15.51</v>
+      </c>
+      <c r="L54" s="5">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="M54" s="5">
+        <v>100</v>
+      </c>
+      <c r="N54" s="5">
+        <v>188</v>
+      </c>
+      <c r="O54" s="5">
+        <v>189536</v>
+      </c>
       <c r="Q54" s="5">
         <v>4</v>
       </c>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
-      <c r="V54" s="5"/>
-      <c r="W54" s="5"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R54" s="5">
+        <v>17193.03</v>
+      </c>
+      <c r="S54" s="5">
+        <v>14.54</v>
+      </c>
+      <c r="T54" s="5">
+        <v>478.6</v>
+      </c>
+      <c r="U54" s="6">
+        <f>100-37/(37+515922)*100</f>
+        <v>99.992828887566645</v>
+      </c>
+      <c r="V54" s="5">
+        <v>186</v>
+      </c>
+      <c r="W54" s="5">
+        <v>208992</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23">
       <c r="A55" s="5">
         <v>5</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="B55" s="5">
+        <v>25451.01</v>
+      </c>
+      <c r="C55" s="5">
+        <v>9.82</v>
+      </c>
+      <c r="D55" s="5">
+        <v>49.88</v>
+      </c>
+      <c r="E55" s="5">
+        <v>100</v>
+      </c>
+      <c r="F55" s="5">
+        <v>93</v>
+      </c>
+      <c r="G55" s="5">
+        <v>66560</v>
+      </c>
       <c r="I55" s="5">
         <v>5</v>
       </c>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
+      <c r="J55" s="5">
+        <v>15924.32</v>
+      </c>
+      <c r="K55" s="5">
+        <v>15.7</v>
+      </c>
+      <c r="L55" s="5">
+        <v>70.459999999999994</v>
+      </c>
+      <c r="M55" s="5">
+        <v>100</v>
+      </c>
+      <c r="N55" s="5">
+        <v>191</v>
+      </c>
+      <c r="O55" s="5">
+        <v>176272</v>
+      </c>
       <c r="Q55" s="5">
         <v>5</v>
       </c>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5"/>
-      <c r="T55" s="5"/>
-      <c r="U55" s="5"/>
-      <c r="V55" s="5"/>
-      <c r="W55" s="5"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R55" s="5">
+        <v>16918.400000000001</v>
+      </c>
+      <c r="S55" s="5">
+        <v>5.55</v>
+      </c>
+      <c r="T55" s="5">
+        <v>492.5</v>
+      </c>
+      <c r="U55" s="6">
+        <f>100-24/(24+507669)*100</f>
+        <v>99.995272733719005</v>
+      </c>
+      <c r="V55" s="5">
+        <v>187</v>
+      </c>
+      <c r="W55" s="5">
+        <v>198144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -4666,12 +4083,12 @@
       <c r="V56" s="5"/>
       <c r="W56" s="5"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -4682,7 +4099,7 @@
         <v>9</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
@@ -4693,7 +4110,7 @@
         <v>9</v>
       </c>
       <c r="R57" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="S57" s="8"/>
       <c r="T57" s="8"/>
@@ -4701,7 +4118,7 @@
       <c r="V57" s="8"/>
       <c r="W57" s="8"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23">
       <c r="A58" s="4">
         <v>500</v>
       </c>
@@ -4766,7 +4183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23">
       <c r="A59" s="5">
         <v>1</v>
       </c>
@@ -4821,7 +4238,7 @@
       <c r="T59" s="5">
         <v>1720</v>
       </c>
-      <c r="U59" s="5">
+      <c r="U59" s="6">
         <v>99.5</v>
       </c>
       <c r="V59" s="5">
@@ -4831,7 +4248,7 @@
         <v>221728</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23">
       <c r="A60" s="5">
         <v>2</v>
       </c>
@@ -4886,7 +4303,7 @@
       <c r="T60" s="5">
         <v>1790</v>
       </c>
-      <c r="U60" s="5">
+      <c r="U60" s="6">
         <v>99.4</v>
       </c>
       <c r="V60" s="5">
@@ -4896,7 +4313,7 @@
         <v>219552</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23">
       <c r="A61" s="5">
         <v>3</v>
       </c>
@@ -4951,7 +4368,7 @@
       <c r="T61" s="5">
         <v>1649</v>
       </c>
-      <c r="U61" s="5">
+      <c r="U61" s="6">
         <v>99.7</v>
       </c>
       <c r="V61" s="5">
@@ -4961,7 +4378,7 @@
         <v>234800</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23">
       <c r="A62" s="5">
         <v>4</v>
       </c>
@@ -5016,7 +4433,7 @@
       <c r="T62" s="5">
         <v>1920</v>
       </c>
-      <c r="U62" s="5">
+      <c r="U62" s="6">
         <v>99.4</v>
       </c>
       <c r="V62" s="5">
@@ -5026,7 +4443,7 @@
         <v>243920</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23">
       <c r="A63" s="5">
         <v>5</v>
       </c>
@@ -5081,7 +4498,7 @@
       <c r="T63" s="5">
         <v>1820</v>
       </c>
-      <c r="U63" s="5">
+      <c r="U63" s="6">
         <v>99.7</v>
       </c>
       <c r="V63" s="5">
@@ -5091,7 +4508,7 @@
         <v>257200</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -5099,12 +4516,12 @@
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23">
       <c r="A65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -5115,7 +4532,7 @@
         <v>9</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
@@ -5126,7 +4543,7 @@
         <v>9</v>
       </c>
       <c r="R65" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="S65" s="8"/>
       <c r="T65" s="8"/>
@@ -5134,7 +4551,7 @@
       <c r="V65" s="8"/>
       <c r="W65" s="8"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23">
       <c r="A66" s="4">
         <v>1000</v>
       </c>
@@ -5157,7 +4574,7 @@
         <v>8</v>
       </c>
       <c r="I66" s="4">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>13</v>
@@ -5178,7 +4595,7 @@
         <v>8</v>
       </c>
       <c r="Q66" s="4">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="R66" s="4" t="s">
         <v>13</v>
@@ -5199,176 +4616,348 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23">
       <c r="A67" s="5">
         <v>1</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
+      <c r="B67" s="5">
+        <v>24846.18</v>
+      </c>
+      <c r="C67" s="5">
+        <v>40.22</v>
+      </c>
+      <c r="D67" s="5">
+        <v>451.41</v>
+      </c>
+      <c r="E67" s="6">
+        <f>100-329/(329+745934)*100</f>
+        <v>99.955913665825591</v>
+      </c>
+      <c r="F67" s="5">
+        <v>91</v>
+      </c>
+      <c r="G67" s="5">
+        <v>68192</v>
+      </c>
       <c r="I67" s="5">
         <v>1</v>
       </c>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="5"/>
+      <c r="J67" s="5">
+        <v>14970.63</v>
+      </c>
+      <c r="K67" s="5">
+        <v>66.75</v>
+      </c>
+      <c r="L67" s="5">
+        <v>511.17</v>
+      </c>
+      <c r="M67" s="6">
+        <f>100-350/(350+449644)*100</f>
+        <v>99.922221185171352</v>
+      </c>
+      <c r="N67" s="5">
+        <v>193</v>
+      </c>
+      <c r="O67" s="5">
+        <v>284000</v>
+      </c>
       <c r="Q67" s="5">
         <v>1</v>
       </c>
-      <c r="R67" s="5"/>
-      <c r="S67" s="5"/>
-      <c r="T67" s="5"/>
-      <c r="U67" s="5"/>
-      <c r="V67" s="5"/>
-      <c r="W67" s="5"/>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R67" s="5">
+        <v>14937.53</v>
+      </c>
+      <c r="S67" s="5">
+        <v>66.91</v>
+      </c>
+      <c r="T67" s="5">
+        <v>6000</v>
+      </c>
+      <c r="U67" s="6">
+        <f>100-580/(580+448210)*100</f>
+        <v>99.870763608814812</v>
+      </c>
+      <c r="V67" s="5">
+        <v>210</v>
+      </c>
+      <c r="W67" s="5">
+        <v>283264</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23">
       <c r="A68" s="5">
         <v>2</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
+      <c r="B68" s="5">
+        <v>24776.04</v>
+      </c>
+      <c r="C68" s="5">
+        <v>40.340000000000003</v>
+      </c>
+      <c r="D68" s="5">
+        <v>466.86</v>
+      </c>
+      <c r="E68" s="6">
+        <f>100-347/(347+743735)*100</f>
+        <v>99.953365354893677</v>
+      </c>
+      <c r="F68">
+        <v>90</v>
+      </c>
+      <c r="G68" s="5">
+        <v>67472</v>
+      </c>
       <c r="I68" s="5">
         <v>2</v>
       </c>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5"/>
+      <c r="J68" s="5">
+        <v>14629.17</v>
+      </c>
+      <c r="K68" s="5">
+        <v>68.36</v>
+      </c>
+      <c r="L68" s="5">
+        <v>452.81</v>
+      </c>
+      <c r="M68" s="6">
+        <f>100-310/(310+439125)*100</f>
+        <v>99.929454868183001</v>
+      </c>
+      <c r="N68" s="5">
+        <v>198</v>
+      </c>
+      <c r="O68" s="5">
+        <v>300096</v>
+      </c>
       <c r="Q68" s="5">
         <v>2</v>
       </c>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
-      <c r="U68" s="5"/>
-      <c r="V68" s="5"/>
-      <c r="W68" s="5"/>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R68" s="5">
+        <v>14518.01</v>
+      </c>
+      <c r="S68" s="5">
+        <v>68.83</v>
+      </c>
+      <c r="T68" s="5">
+        <v>5140</v>
+      </c>
+      <c r="U68" s="6">
+        <f>100-2256/(2556+434115)*100</f>
+        <v>99.483363905549027</v>
+      </c>
+      <c r="V68" s="5">
+        <v>206</v>
+      </c>
+      <c r="W68" s="5">
+        <v>366512</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23">
       <c r="A69" s="5">
         <v>3</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
+      <c r="B69" s="5">
+        <v>24789.88</v>
+      </c>
+      <c r="C69" s="5">
+        <v>40.380000000000003</v>
+      </c>
+      <c r="D69" s="5">
+        <v>479.3</v>
+      </c>
+      <c r="E69" s="6">
+        <f>100-341/(744119+341)*100</f>
+        <v>99.954194986970421</v>
+      </c>
+      <c r="F69" s="5">
+        <v>91</v>
+      </c>
+      <c r="G69" s="5">
+        <v>67280</v>
+      </c>
       <c r="I69" s="5">
         <v>3</v>
       </c>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
+      <c r="J69" s="5">
+        <v>14524.19</v>
+      </c>
+      <c r="K69" s="5">
+        <v>68.75</v>
+      </c>
+      <c r="L69" s="5">
+        <v>594.74</v>
+      </c>
+      <c r="M69" s="6">
+        <f>100-350/(350+436354)*100</f>
+        <v>99.919854180405949</v>
+      </c>
+      <c r="N69" s="5">
+        <v>195</v>
+      </c>
+      <c r="O69" s="5">
+        <v>286704</v>
+      </c>
       <c r="Q69" s="5">
         <v>3</v>
       </c>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R69" s="5">
+        <v>14594.26</v>
+      </c>
+      <c r="S69" s="5">
+        <v>67.849999999999994</v>
+      </c>
+      <c r="T69" s="5">
+        <v>4350</v>
+      </c>
+      <c r="U69" s="6">
+        <f>100-2366/(2366+436629)*100</f>
+        <v>99.461041697513636</v>
+      </c>
+      <c r="V69" s="5">
+        <v>203</v>
+      </c>
+      <c r="W69" s="5">
+        <v>317392</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23">
       <c r="A70" s="5">
         <v>4</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
+      <c r="B70" s="5">
+        <v>24746.3</v>
+      </c>
+      <c r="C70" s="5">
+        <v>40.380000000000003</v>
+      </c>
+      <c r="D70" s="5">
+        <v>479.3</v>
+      </c>
+      <c r="E70" s="6">
+        <f>100-322/(322+742886)*100</f>
+        <v>99.956674309210882</v>
+      </c>
+      <c r="F70" s="5">
+        <v>90</v>
+      </c>
+      <c r="G70" s="5">
+        <v>6824</v>
+      </c>
       <c r="I70" s="5">
         <v>4</v>
       </c>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5"/>
+      <c r="J70" s="5">
+        <v>14274.59</v>
+      </c>
+      <c r="K70" s="5">
+        <v>69.98</v>
+      </c>
+      <c r="L70" s="5">
+        <v>572.30999999999995</v>
+      </c>
+      <c r="M70" s="6">
+        <f>100-337/(337+428541)*100</f>
+        <v>99.921422875503055</v>
+      </c>
+      <c r="N70" s="5">
+        <v>199</v>
+      </c>
+      <c r="O70" s="5">
+        <v>294704</v>
+      </c>
       <c r="Q70" s="5">
         <v>4</v>
       </c>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
-      <c r="U70" s="5"/>
-      <c r="V70" s="5"/>
-      <c r="W70" s="5"/>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R70" s="5">
+        <v>14719.55</v>
+      </c>
+      <c r="S70" s="5">
+        <v>68.2</v>
+      </c>
+      <c r="T70" s="5">
+        <v>4540</v>
+      </c>
+      <c r="U70" s="6">
+        <f>100-2739/(2739+439861)*100</f>
+        <v>99.381156800723005</v>
+      </c>
+      <c r="V70" s="5">
+        <v>198</v>
+      </c>
+      <c r="W70" s="5">
+        <v>361280</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23">
       <c r="A71" s="5">
         <v>5</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
+      <c r="B71" s="5">
+        <v>24773.9</v>
+      </c>
+      <c r="C71" s="5">
+        <v>40.340000000000003</v>
+      </c>
+      <c r="D71" s="5">
+        <v>462.65</v>
+      </c>
+      <c r="E71" s="6">
+        <f>100-321/(321+743725)*100</f>
+        <v>99.956857506121935</v>
+      </c>
+      <c r="F71" s="5">
+        <v>91</v>
+      </c>
+      <c r="G71" s="5">
+        <v>67952</v>
+      </c>
       <c r="I71" s="5">
         <v>5</v>
       </c>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="5"/>
-      <c r="N71" s="5"/>
-      <c r="O71" s="5"/>
+      <c r="J71" s="5">
+        <v>13378.25</v>
+      </c>
+      <c r="K71" s="5">
+        <v>74.77</v>
+      </c>
+      <c r="L71" s="5">
+        <v>550.02</v>
+      </c>
+      <c r="M71" s="6">
+        <f>100-336/(336+401120)*100</f>
+        <v>99.916304651070107</v>
+      </c>
+      <c r="N71" s="5">
+        <v>190</v>
+      </c>
+      <c r="O71" s="5">
+        <v>311296</v>
+      </c>
       <c r="Q71" s="5">
         <v>5</v>
       </c>
-      <c r="R71" s="5"/>
-      <c r="S71" s="5"/>
-      <c r="T71" s="5"/>
-      <c r="U71" s="5"/>
-      <c r="V71" s="5"/>
-      <c r="W71" s="5"/>
+      <c r="R71" s="5">
+        <v>14651.76</v>
+      </c>
+      <c r="S71" s="5">
+        <v>68.2</v>
+      </c>
+      <c r="T71" s="5">
+        <v>4540</v>
+      </c>
+      <c r="U71" s="3">
+        <f>100-2214/(2214+438230)*100</f>
+        <v>99.49732542616087</v>
+      </c>
+      <c r="V71" s="5">
+        <v>206</v>
+      </c>
+      <c r="W71" s="5">
+        <v>323952</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="J57:O57"/>
-    <mergeCell ref="R57:W57"/>
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="J65:O65"/>
-    <mergeCell ref="R65:W65"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="J41:O41"/>
-    <mergeCell ref="R41:W41"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="J49:O49"/>
-    <mergeCell ref="R49:W49"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="R30:W30"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="I40:O40"/>
-    <mergeCell ref="Q40:W40"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="R14:W14"/>
     <mergeCell ref="R22:W22"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B14:G14"/>
@@ -5376,13 +4965,36 @@
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="J14:O14"/>
     <mergeCell ref="J22:O22"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="R14:W14"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="R30:W30"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="I40:O40"/>
+    <mergeCell ref="Q40:W40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="J41:O41"/>
+    <mergeCell ref="R41:W41"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="J49:O49"/>
+    <mergeCell ref="R49:W49"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="J57:O57"/>
+    <mergeCell ref="R57:W57"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="J65:O65"/>
+    <mergeCell ref="R65:W65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E6FA74-58D8-2745-A48E-13C60CDE5766}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -5390,13 +5002,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -5404,7 +5016,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -5412,7 +5024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5423,7 +5035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5434,7 +5046,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5445,7 +5057,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5456,7 +5068,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -5467,7 +5079,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5478,7 +5090,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -5486,7 +5098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -5497,7 +5109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5508,7 +5120,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -5519,7 +5131,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -5530,7 +5142,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -5541,7 +5153,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -5552,7 +5164,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -5560,7 +5172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -5571,7 +5183,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5582,7 +5194,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -5593,7 +5205,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -5604,7 +5216,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -5615,7 +5227,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -5630,4 +5242,970 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506776CC-B6C8-BB4A-88D0-81938826640D}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>500</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>23707.59</v>
+      </c>
+      <c r="C8">
+        <v>21.08</v>
+      </c>
+      <c r="D8">
+        <v>195.63</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>90</v>
+      </c>
+      <c r="G8">
+        <v>64264</v>
+      </c>
+      <c r="H8" s="2">
+        <v>23899.18</v>
+      </c>
+      <c r="I8" s="6">
+        <v>20.91</v>
+      </c>
+      <c r="J8" s="6">
+        <v>116.19</v>
+      </c>
+      <c r="K8" s="5">
+        <v>100</v>
+      </c>
+      <c r="L8" s="5">
+        <v>96</v>
+      </c>
+      <c r="M8" s="5">
+        <v>82128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5">
+        <v>23920.81</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20.9</v>
+      </c>
+      <c r="D9" s="5">
+        <v>239.5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>100</v>
+      </c>
+      <c r="F9" s="5">
+        <v>86</v>
+      </c>
+      <c r="G9" s="5">
+        <v>65040</v>
+      </c>
+      <c r="H9" s="5">
+        <v>24201.74</v>
+      </c>
+      <c r="I9" s="5">
+        <v>20.65</v>
+      </c>
+      <c r="J9" s="5">
+        <v>108.4</v>
+      </c>
+      <c r="K9" s="5">
+        <v>100</v>
+      </c>
+      <c r="L9" s="5">
+        <v>96</v>
+      </c>
+      <c r="M9" s="5">
+        <v>83196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5">
+        <v>23909.89</v>
+      </c>
+      <c r="C10" s="5">
+        <v>20.9</v>
+      </c>
+      <c r="D10" s="5">
+        <v>204.46</v>
+      </c>
+      <c r="E10" s="5">
+        <v>100</v>
+      </c>
+      <c r="F10" s="5">
+        <v>90</v>
+      </c>
+      <c r="G10" s="5">
+        <v>65024</v>
+      </c>
+      <c r="H10" s="5">
+        <v>24153.93</v>
+      </c>
+      <c r="I10" s="5">
+        <v>20.69</v>
+      </c>
+      <c r="J10" s="5">
+        <v>115.38</v>
+      </c>
+      <c r="K10" s="5">
+        <v>100</v>
+      </c>
+      <c r="L10" s="5">
+        <v>100</v>
+      </c>
+      <c r="M10" s="5">
+        <v>82692</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5">
+        <v>23825.78</v>
+      </c>
+      <c r="C11" s="5">
+        <v>20.98</v>
+      </c>
+      <c r="D11" s="5">
+        <v>206.59</v>
+      </c>
+      <c r="E11" s="5">
+        <v>100</v>
+      </c>
+      <c r="F11" s="5">
+        <v>89</v>
+      </c>
+      <c r="G11" s="5">
+        <v>64880</v>
+      </c>
+      <c r="H11" s="5">
+        <v>23658.7</v>
+      </c>
+      <c r="I11" s="5">
+        <v>21.12</v>
+      </c>
+      <c r="J11" s="5">
+        <v>119.64</v>
+      </c>
+      <c r="K11" s="5">
+        <v>100</v>
+      </c>
+      <c r="L11" s="5">
+        <v>98</v>
+      </c>
+      <c r="M11" s="5">
+        <v>82672</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5">
+        <v>23879.56</v>
+      </c>
+      <c r="C12" s="5">
+        <v>20.93</v>
+      </c>
+      <c r="D12" s="5">
+        <v>220.08</v>
+      </c>
+      <c r="E12" s="5">
+        <v>100</v>
+      </c>
+      <c r="F12" s="5">
+        <v>90</v>
+      </c>
+      <c r="G12" s="5">
+        <v>64880</v>
+      </c>
+      <c r="H12" s="5">
+        <v>24399.08</v>
+      </c>
+      <c r="I12" s="5">
+        <v>20.5</v>
+      </c>
+      <c r="J12" s="5">
+        <v>117.62</v>
+      </c>
+      <c r="K12" s="5">
+        <v>100</v>
+      </c>
+      <c r="L12" s="5">
+        <v>99</v>
+      </c>
+      <c r="M12" s="5">
+        <v>82948</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
+        <v>24363.11</v>
+      </c>
+      <c r="I13" s="5">
+        <v>20.51</v>
+      </c>
+      <c r="J13" s="5">
+        <v>120.77</v>
+      </c>
+      <c r="K13" s="5">
+        <v>100</v>
+      </c>
+      <c r="L13" s="5">
+        <v>99</v>
+      </c>
+      <c r="M13" s="5">
+        <v>84116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5">
+        <v>14317.65</v>
+      </c>
+      <c r="C16" s="5">
+        <v>34.93</v>
+      </c>
+      <c r="D16" s="5">
+        <v>248.08</v>
+      </c>
+      <c r="E16" s="5">
+        <v>100</v>
+      </c>
+      <c r="F16" s="5">
+        <v>189</v>
+      </c>
+      <c r="G16" s="5">
+        <v>229776</v>
+      </c>
+      <c r="H16" s="5">
+        <v>7650.31</v>
+      </c>
+      <c r="I16" s="5">
+        <v>64.53</v>
+      </c>
+      <c r="J16" s="5">
+        <v>287.7</v>
+      </c>
+      <c r="K16" s="5">
+        <v>100</v>
+      </c>
+      <c r="L16" s="5">
+        <v>166</v>
+      </c>
+      <c r="M16" s="5">
+        <v>105356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5">
+        <v>14508.2</v>
+      </c>
+      <c r="C17" s="5">
+        <v>34.46</v>
+      </c>
+      <c r="D17" s="5">
+        <v>231.62</v>
+      </c>
+      <c r="E17" s="5">
+        <v>100</v>
+      </c>
+      <c r="F17" s="5">
+        <v>197</v>
+      </c>
+      <c r="G17" s="5">
+        <v>198496</v>
+      </c>
+      <c r="H17" s="5">
+        <v>8460.4599999999991</v>
+      </c>
+      <c r="I17" s="5">
+        <v>58.41</v>
+      </c>
+      <c r="J17" s="5">
+        <v>305.45999999999998</v>
+      </c>
+      <c r="K17" s="5">
+        <v>100</v>
+      </c>
+      <c r="L17" s="5">
+        <v>176</v>
+      </c>
+      <c r="M17" s="5">
+        <v>106928</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5">
+        <v>14466.72</v>
+      </c>
+      <c r="C18" s="5">
+        <v>34.56</v>
+      </c>
+      <c r="D18" s="5">
+        <v>214.82</v>
+      </c>
+      <c r="E18" s="5">
+        <v>100</v>
+      </c>
+      <c r="F18" s="5">
+        <v>185</v>
+      </c>
+      <c r="G18" s="5">
+        <v>208496</v>
+      </c>
+      <c r="H18" s="5">
+        <v>8428.35</v>
+      </c>
+      <c r="I18" s="5">
+        <v>58.51</v>
+      </c>
+      <c r="J18" s="5">
+        <v>285.69</v>
+      </c>
+      <c r="K18" s="5">
+        <v>100</v>
+      </c>
+      <c r="L18" s="5">
+        <v>166</v>
+      </c>
+      <c r="M18" s="5">
+        <v>103704</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5">
+        <v>14610.55</v>
+      </c>
+      <c r="C19" s="5">
+        <v>34.21</v>
+      </c>
+      <c r="D19" s="5">
+        <v>198.59</v>
+      </c>
+      <c r="E19" s="5">
+        <v>100</v>
+      </c>
+      <c r="F19" s="5">
+        <v>176</v>
+      </c>
+      <c r="G19" s="5">
+        <v>212880</v>
+      </c>
+      <c r="H19" s="5">
+        <v>8292.3700000000008</v>
+      </c>
+      <c r="I19" s="5">
+        <v>59.61</v>
+      </c>
+      <c r="J19" s="5">
+        <v>313.20999999999998</v>
+      </c>
+      <c r="K19" s="5">
+        <v>100</v>
+      </c>
+      <c r="L19" s="5">
+        <v>171</v>
+      </c>
+      <c r="M19" s="5">
+        <v>106108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5">
+        <v>14647.9</v>
+      </c>
+      <c r="C20" s="5">
+        <v>34.119999999999997</v>
+      </c>
+      <c r="D20" s="5">
+        <v>238.61</v>
+      </c>
+      <c r="E20" s="5">
+        <v>100</v>
+      </c>
+      <c r="F20" s="5">
+        <v>190</v>
+      </c>
+      <c r="G20" s="5">
+        <v>209896</v>
+      </c>
+      <c r="H20" s="5">
+        <v>8410.83</v>
+      </c>
+      <c r="I20" s="5">
+        <v>58.73</v>
+      </c>
+      <c r="J20" s="5">
+        <v>292.88</v>
+      </c>
+      <c r="K20" s="5">
+        <v>100</v>
+      </c>
+      <c r="L20" s="5">
+        <v>165</v>
+      </c>
+      <c r="M20" s="5">
+        <v>104264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="5">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <v>14790.27</v>
+      </c>
+      <c r="C24" s="5">
+        <v>33.81</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1720</v>
+      </c>
+      <c r="E24" s="5">
+        <v>99.5</v>
+      </c>
+      <c r="F24" s="5">
+        <v>195</v>
+      </c>
+      <c r="G24" s="5">
+        <v>221728</v>
+      </c>
+      <c r="H24" s="5">
+        <v>10322.75</v>
+      </c>
+      <c r="I24" s="5">
+        <v>47.96</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1710</v>
+      </c>
+      <c r="K24" s="5">
+        <v>100</v>
+      </c>
+      <c r="L24" s="5">
+        <v>268</v>
+      </c>
+      <c r="M24" s="5">
+        <v>172996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="5">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5">
+        <v>14729.2</v>
+      </c>
+      <c r="C25" s="5">
+        <v>33.93</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1790</v>
+      </c>
+      <c r="E25" s="5">
+        <v>99.4</v>
+      </c>
+      <c r="F25" s="5">
+        <v>194</v>
+      </c>
+      <c r="G25" s="5">
+        <v>219552</v>
+      </c>
+      <c r="H25" s="5">
+        <v>10462.030000000001</v>
+      </c>
+      <c r="I25" s="5">
+        <v>47.33</v>
+      </c>
+      <c r="J25" s="5">
+        <v>1740</v>
+      </c>
+      <c r="K25" s="5">
+        <v>100</v>
+      </c>
+      <c r="L25" s="5">
+        <v>265</v>
+      </c>
+      <c r="M25" s="5">
+        <v>118604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="5">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5">
+        <v>14749.95</v>
+      </c>
+      <c r="C26" s="5">
+        <v>33.909999999999997</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1649</v>
+      </c>
+      <c r="E26" s="5">
+        <v>99.7</v>
+      </c>
+      <c r="F26" s="5">
+        <v>198</v>
+      </c>
+      <c r="G26" s="5">
+        <v>234800</v>
+      </c>
+      <c r="H26" s="5">
+        <v>10337.76</v>
+      </c>
+      <c r="I26" s="5">
+        <v>47.97</v>
+      </c>
+      <c r="J26" s="5">
+        <v>1770</v>
+      </c>
+      <c r="K26" s="5">
+        <v>100</v>
+      </c>
+      <c r="L26" s="5">
+        <v>250</v>
+      </c>
+      <c r="M26" s="5">
+        <v>174576</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="5">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5">
+        <v>14722.22</v>
+      </c>
+      <c r="C27" s="5">
+        <v>33.979999999999997</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1920</v>
+      </c>
+      <c r="E27" s="5">
+        <v>99.4</v>
+      </c>
+      <c r="F27" s="5">
+        <v>193</v>
+      </c>
+      <c r="G27" s="5">
+        <v>243920</v>
+      </c>
+      <c r="H27" s="5">
+        <v>10478.85</v>
+      </c>
+      <c r="I27" s="5">
+        <v>47.32</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1740</v>
+      </c>
+      <c r="K27" s="5">
+        <v>100</v>
+      </c>
+      <c r="L27" s="5">
+        <v>264</v>
+      </c>
+      <c r="M27" s="5">
+        <v>175628</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="5">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5">
+        <v>14628.28</v>
+      </c>
+      <c r="C28" s="5">
+        <v>34.14</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1820</v>
+      </c>
+      <c r="E28" s="5">
+        <v>99.7</v>
+      </c>
+      <c r="F28" s="5">
+        <v>194</v>
+      </c>
+      <c r="G28" s="5">
+        <v>257200</v>
+      </c>
+      <c r="H28" s="5">
+        <v>10254</v>
+      </c>
+      <c r="I28" s="5">
+        <v>48.39</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1740</v>
+      </c>
+      <c r="K28" s="5">
+        <v>100</v>
+      </c>
+      <c r="L28" s="5">
+        <v>262</v>
+      </c>
+      <c r="M28" s="5">
+        <v>175036</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="H22:M22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(benchmarks): update fibonacci to use number 45
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksOverview.xlsx
+++ b/benchmarks/BenchmarksOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF6B1F4-20D1-40B4-A48B-99C2148CCD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0301B95C-F737-4E72-99C2-C9304752AD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic HTTP Server" sheetId="1" r:id="rId1"/>
@@ -1333,7 +1333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB541521-64F8-DE46-A0B5-E150B1049D8B}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="87" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
@@ -4998,8 +4998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E6FA74-58D8-2745-A48E-13C60CDE5766}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -5013,7 +5013,7 @@
         <v>15</v>
       </c>
       <c r="B1">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5040,7 +5040,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.31</v>
+        <v>3.21</v>
       </c>
       <c r="C5">
         <v>0.41</v>
@@ -5051,7 +5051,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0.31</v>
+        <v>3.21</v>
       </c>
       <c r="C6">
         <v>0.41</v>
@@ -5062,7 +5062,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.31</v>
+        <v>3.21</v>
       </c>
       <c r="C7">
         <v>0.4</v>
@@ -5073,7 +5073,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.31</v>
+        <v>3.22</v>
       </c>
       <c r="C8">
         <v>0.42</v>
@@ -5084,7 +5084,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.31</v>
+        <v>3.21</v>
       </c>
       <c r="C9">
         <v>0.42</v>
@@ -5114,7 +5114,7 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>0.62</v>
+        <v>6.46</v>
       </c>
       <c r="C13">
         <v>0.68</v>
@@ -5125,7 +5125,7 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>0.62</v>
+        <v>6.47</v>
       </c>
       <c r="C14">
         <v>0.68</v>
@@ -5136,7 +5136,7 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>0.62</v>
+        <v>6.46</v>
       </c>
       <c r="C15">
         <v>0.69</v>
@@ -5147,7 +5147,7 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>0.62</v>
+        <v>6.46</v>
       </c>
       <c r="C16">
         <v>0.67</v>
@@ -5158,7 +5158,7 @@
         <v>5</v>
       </c>
       <c r="B17">
-        <v>0.62</v>
+        <v>6.46</v>
       </c>
       <c r="C17">
         <v>0.69</v>
@@ -5174,7 +5174,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -5188,7 +5188,7 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>0.6</v>
+        <v>6.3</v>
       </c>
       <c r="C21">
         <v>0.66</v>
@@ -5199,7 +5199,7 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>0.6</v>
+        <v>6.3</v>
       </c>
       <c r="C22">
         <v>0.67</v>
@@ -5210,7 +5210,7 @@
         <v>3</v>
       </c>
       <c r="B23">
-        <v>0.6</v>
+        <v>6.3</v>
       </c>
       <c r="C23">
         <v>0.67</v>
@@ -5221,7 +5221,7 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>0.6</v>
+        <v>6.29</v>
       </c>
       <c r="C24">
         <v>0.67</v>
@@ -5232,7 +5232,7 @@
         <v>5</v>
       </c>
       <c r="B25">
-        <v>0.6</v>
+        <v>6.29</v>
       </c>
       <c r="C25">
         <v>0.69</v>

</xml_diff>

<commit_message>
feat: Review & Anhang
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksOverview.xlsx
+++ b/benchmarks/BenchmarksOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CAF16A-D7A7-4C79-85E1-EB36B4A30C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA92A643-5616-4555-BE1F-B51F814C90AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="HTTP-Server" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -178,6 +178,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -494,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E627F5D-FFE4-2643-9D4B-9E18438983C0}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1514,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB541521-64F8-DE46-A0B5-E150B1049D8B}">
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="87" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:O15"/>
+    <sheetView topLeftCell="A52" zoomScale="87" workbookViewId="0">
+      <selection activeCell="W85" sqref="W85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -3743,16 +3744,15 @@
       <c r="W44" s="8"/>
     </row>
     <row r="48" spans="1:23">
-      <c r="A48" s="9" t="s">
+      <c r="B48" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
+      <c r="H48" s="11"/>
       <c r="I48" s="9" t="s">
         <v>3</v>
       </c>
@@ -5880,29 +5880,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="J67:O67"/>
-    <mergeCell ref="R67:W67"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="J76:O76"/>
-    <mergeCell ref="R76:W76"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="J49:O49"/>
-    <mergeCell ref="R49:W49"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="J58:O58"/>
-    <mergeCell ref="R58:W58"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="J34:O34"/>
-    <mergeCell ref="R34:W34"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="I48:O48"/>
-    <mergeCell ref="Q48:W48"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="R15:W15"/>
     <mergeCell ref="R24:W24"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B15:G15"/>
@@ -5910,6 +5887,29 @@
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="J15:O15"/>
     <mergeCell ref="J24:O24"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="R15:W15"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="J34:O34"/>
+    <mergeCell ref="R34:W34"/>
+    <mergeCell ref="I48:O48"/>
+    <mergeCell ref="Q48:W48"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="J49:O49"/>
+    <mergeCell ref="R49:W49"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="J58:O58"/>
+    <mergeCell ref="R58:W58"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="J67:O67"/>
+    <mergeCell ref="R67:W67"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="J76:O76"/>
+    <mergeCell ref="R76:W76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5921,7 +5921,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:J12"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
fix: Wiederholen der falschen Header in Longtable
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksOverview.xlsx
+++ b/benchmarks/BenchmarksOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA92A643-5616-4555-BE1F-B51F814C90AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755CCBBE-539C-4427-BF1C-BCA8EEFBC76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="HTTP-Server" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -178,7 +178,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -495,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E627F5D-FFE4-2643-9D4B-9E18438983C0}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1515,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB541521-64F8-DE46-A0B5-E150B1049D8B}">
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="87" workbookViewId="0">
-      <selection activeCell="W85" sqref="W85"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="87" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -3752,7 +3751,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="11"/>
+      <c r="H48" s="1"/>
       <c r="I48" s="9" t="s">
         <v>3</v>
       </c>
@@ -4804,7 +4803,7 @@
         <v>476.096</v>
       </c>
       <c r="U65" s="8">
-        <f t="shared" si="65"/>
+        <f>AVERAGE(U60:U64)</f>
         <v>99.99316553128449</v>
       </c>
       <c r="V65" s="8">
@@ -5880,6 +5879,29 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="J67:O67"/>
+    <mergeCell ref="R67:W67"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="J76:O76"/>
+    <mergeCell ref="R76:W76"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="J49:O49"/>
+    <mergeCell ref="R49:W49"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="J58:O58"/>
+    <mergeCell ref="R58:W58"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="J34:O34"/>
+    <mergeCell ref="R34:W34"/>
+    <mergeCell ref="I48:O48"/>
+    <mergeCell ref="Q48:W48"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="R15:W15"/>
     <mergeCell ref="R24:W24"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B15:G15"/>
@@ -5887,29 +5909,6 @@
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="J15:O15"/>
     <mergeCell ref="J24:O24"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="R15:W15"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="J34:O34"/>
-    <mergeCell ref="R34:W34"/>
-    <mergeCell ref="I48:O48"/>
-    <mergeCell ref="Q48:W48"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="J49:O49"/>
-    <mergeCell ref="R49:W49"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="J58:O58"/>
-    <mergeCell ref="R58:W58"/>
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="J67:O67"/>
-    <mergeCell ref="R67:W67"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="J76:O76"/>
-    <mergeCell ref="R76:W76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5920,8 +5919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E6FA74-58D8-2745-A48E-13C60CDE5766}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
fix: Unterschiede in Testdaten zw. Anhang und Excel
</commit_message>
<xml_diff>
--- a/benchmarks/BenchmarksOverview.xlsx
+++ b/benchmarks/BenchmarksOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansgar\Documents\Development\Repositories\BunVsNodeJs\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755CCBBE-539C-4427-BF1C-BCA8EEFBC76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1005A9BC-E3F7-462E-A6BE-80FA8D930F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3EB33065-7B02-8F40-AA24-6363AD3E5C2F}"/>
   </bookViews>
@@ -142,12 +142,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -178,6 +184,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1514,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB541521-64F8-DE46-A0B5-E150B1049D8B}">
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="87" workbookViewId="0">
-      <selection activeCell="T43" sqref="T43"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -4150,8 +4158,8 @@
       <c r="F55" s="5">
         <v>94</v>
       </c>
-      <c r="G55" s="5">
-        <v>654230</v>
+      <c r="G55" s="11">
+        <v>65423</v>
       </c>
       <c r="I55" s="5">
         <v>5</v>
@@ -4220,9 +4228,9 @@
         <f t="shared" si="60"/>
         <v>93.6</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="12">
         <f t="shared" si="60"/>
-        <v>183819.6</v>
+        <v>66058.2</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>18</v>
@@ -5678,8 +5686,8 @@
       <c r="F81" s="5">
         <v>90</v>
       </c>
-      <c r="G81" s="5">
-        <v>6824</v>
+      <c r="G81" s="11">
+        <v>68240</v>
       </c>
       <c r="I81" s="5">
         <v>4</v>
@@ -5818,9 +5826,9 @@
         <f t="shared" si="69"/>
         <v>90.6</v>
       </c>
-      <c r="G83" s="8">
+      <c r="G83" s="12">
         <f t="shared" si="69"/>
-        <v>55544</v>
+        <v>67827.199999999997</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>18</v>
@@ -5879,29 +5887,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="J67:O67"/>
-    <mergeCell ref="R67:W67"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="J76:O76"/>
-    <mergeCell ref="R76:W76"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="J49:O49"/>
-    <mergeCell ref="R49:W49"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="J58:O58"/>
-    <mergeCell ref="R58:W58"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="J34:O34"/>
-    <mergeCell ref="R34:W34"/>
-    <mergeCell ref="I48:O48"/>
-    <mergeCell ref="Q48:W48"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="R6:W6"/>
-    <mergeCell ref="R15:W15"/>
     <mergeCell ref="R24:W24"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B15:G15"/>
@@ -5909,6 +5894,29 @@
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="J15:O15"/>
     <mergeCell ref="J24:O24"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="R6:W6"/>
+    <mergeCell ref="R15:W15"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="J34:O34"/>
+    <mergeCell ref="R34:W34"/>
+    <mergeCell ref="I48:O48"/>
+    <mergeCell ref="Q48:W48"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="J49:O49"/>
+    <mergeCell ref="R49:W49"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="J58:O58"/>
+    <mergeCell ref="R58:W58"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="J67:O67"/>
+    <mergeCell ref="R67:W67"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="J76:O76"/>
+    <mergeCell ref="R76:W76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>